<commit_message>
Flugbahnen angepasst. Neue Pizzasymbole. Erweiterungen im XML erfasst. Kommentare erfasst.
</commit_message>
<xml_diff>
--- a/LiesMich.xlsx
+++ b/LiesMich.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago.freitas\Documents\20201020\Morgen\NoFood4USolution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GD\private\AZW\Lehrlingswettbewerb\2023\kurt\20231023\Abend\NoFood4USolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B231B4-1B1E-45EC-8B1C-2A7202189016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCF1AF3-8B18-415C-BD7E-3C7BEF4E7AB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,28 +16,19 @@
     <sheet name="Entwicklung" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Entwicklung!$A$1:$I$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Entwicklung!$A$1:$I$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="44">
   <si>
     <t>#</t>
   </si>
@@ -126,9 +117,6 @@
     <t>Hitbox wird gelöscht nach dem Tod</t>
   </si>
   <si>
-    <t>Restart Button</t>
-  </si>
-  <si>
     <t>Tiago oder so</t>
   </si>
   <si>
@@ -157,6 +145,21 @@
   </si>
   <si>
     <t>Beim Aufstarten zufällige Flugbahnen automatisch auswählen</t>
+  </si>
+  <si>
+    <t>Wenn ein Insekt über das Essen fliegt soll ein Geräusch entstehen, z.B. Rülpsen</t>
+  </si>
+  <si>
+    <t>Restart Button, ESC-Button.</t>
+  </si>
+  <si>
+    <t>Insektensummgeräusch</t>
+  </si>
+  <si>
+    <t>Wenn auf das Essen geklickt wird, soll GameOver erscheinen</t>
+  </si>
+  <si>
+    <t>Essen soll nach jedem Insektenüberflug, stückweise kleiner werden.</t>
   </si>
 </sst>
 </file>
@@ -529,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +797,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>4</v>
@@ -803,7 +806,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -811,7 +817,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
@@ -821,6 +827,9 @@
       </c>
       <c r="E15" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -828,7 +837,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>4</v>
@@ -840,12 +849,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>4</v>
@@ -857,12 +866,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>4</v>
@@ -874,12 +883,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>4</v>
@@ -891,12 +900,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>4</v>
@@ -908,12 +917,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>4</v>
@@ -925,15 +934,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>23</v>
@@ -941,16 +950,19 @@
       <c r="E22" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>23</v>
@@ -958,9 +970,68 @@
       <c r="E23" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F23" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I14" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I26" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>